<commit_message>
Checklist & font update
</commit_message>
<xml_diff>
--- a/Planning/3D Checklist.xlsx
+++ b/Planning/3D Checklist.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="91">
   <si>
     <t>Assets</t>
   </si>
@@ -289,6 +289,9 @@
   </si>
   <si>
     <t>need to sync</t>
+  </si>
+  <si>
+    <t>yes</t>
   </si>
 </sst>
 </file>
@@ -683,8 +686,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D69" sqref="D69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1164,6 +1167,12 @@
         <v>10</v>
       </c>
       <c r="B68" s="2"/>
+      <c r="C68" t="s">
+        <v>90</v>
+      </c>
+      <c r="D68" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
@@ -1250,6 +1259,9 @@
         <v>84</v>
       </c>
       <c r="B81" s="2"/>
+      <c r="C81" t="s">
+        <v>90</v>
+      </c>
       <c r="D81" t="s">
         <v>83</v>
       </c>

</xml_diff>

<commit_message>
rescale gefixed en afgefinkt
mijn objecten zijn af
</commit_message>
<xml_diff>
--- a/Planning/3D Checklist.xlsx
+++ b/Planning/3D Checklist.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="94">
   <si>
     <t>Assets</t>
   </si>
@@ -303,6 +303,9 @@
   </si>
   <si>
     <t>need to export</t>
+  </si>
+  <si>
+    <t>lara</t>
   </si>
 </sst>
 </file>
@@ -716,8 +719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C78" sqref="C78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -828,6 +831,12 @@
         <v>5</v>
       </c>
       <c r="B13" s="2"/>
+      <c r="C13" t="s">
+        <v>88</v>
+      </c>
+      <c r="D13" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -927,12 +936,30 @@
         <v>25</v>
       </c>
       <c r="B22" s="2"/>
+      <c r="C22" t="s">
+        <v>88</v>
+      </c>
+      <c r="D22" t="s">
+        <v>93</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B23" s="2"/>
+      <c r="C23" t="s">
+        <v>88</v>
+      </c>
+      <c r="D23" t="s">
+        <v>93</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
@@ -1004,7 +1031,10 @@
       <c r="A30" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B30" s="3"/>
+      <c r="B30" s="2"/>
+      <c r="C30" t="s">
+        <v>88</v>
+      </c>
       <c r="D30" t="s">
         <v>91</v>
       </c>
@@ -1030,25 +1060,25 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B33" s="3"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B34" s="3"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>69</v>
       </c>
       <c r="B35" s="2"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>68</v>
       </c>
@@ -1057,19 +1087,19 @@
         <v>85</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B37" s="3"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>71</v>
       </c>
       <c r="B38" s="2"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>30</v>
       </c>
@@ -1078,136 +1108,199 @@
         <v>91</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>61</v>
       </c>
       <c r="B40" s="3"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>60</v>
       </c>
       <c r="B41" s="3"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B42" s="2"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B43" s="2"/>
+      <c r="C43" t="s">
+        <v>88</v>
+      </c>
       <c r="D43" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B44" s="3"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B45" s="3"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B46" s="3"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>80</v>
       </c>
       <c r="B47" s="2"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>88</v>
+      </c>
+      <c r="D47" t="s">
+        <v>93</v>
+      </c>
+      <c r="E47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>76</v>
       </c>
       <c r="B48" s="2"/>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>88</v>
+      </c>
+      <c r="D48" t="s">
+        <v>93</v>
+      </c>
+      <c r="E48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>77</v>
       </c>
       <c r="B49" s="2"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>88</v>
+      </c>
+      <c r="D49" t="s">
+        <v>93</v>
+      </c>
+      <c r="E49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>78</v>
       </c>
       <c r="B50" s="2"/>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
+        <v>88</v>
+      </c>
+      <c r="D50" t="s">
+        <v>93</v>
+      </c>
+      <c r="E50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>79</v>
       </c>
       <c r="B51" s="2"/>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
+        <v>88</v>
+      </c>
+      <c r="D51" t="s">
+        <v>93</v>
+      </c>
+      <c r="E51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B52" s="3"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B53" s="3"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B54" s="2"/>
+      <c r="C54" t="s">
+        <v>88</v>
+      </c>
       <c r="D54" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B55" s="3"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B56" s="3"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B57" s="3"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B58" s="2"/>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C58" t="s">
+        <v>88</v>
+      </c>
+      <c r="D58" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B59" s="3"/>
+      <c r="B59" s="2"/>
+      <c r="C59" t="s">
+        <v>88</v>
+      </c>
       <c r="D59" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>9</v>
       </c>
@@ -1219,25 +1312,25 @@
         <v>82</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B61" s="3"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B62" s="3"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>55</v>
       </c>
       <c r="B63" s="3"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>38</v>
       </c>
@@ -1247,7 +1340,13 @@
       <c r="A65" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B65" s="3"/>
+      <c r="B65" s="2"/>
+      <c r="C65" t="s">
+        <v>88</v>
+      </c>
+      <c r="D65" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
@@ -1260,6 +1359,9 @@
         <v>16</v>
       </c>
       <c r="B67" s="2"/>
+      <c r="C67" t="s">
+        <v>88</v>
+      </c>
       <c r="D67" t="s">
         <v>91</v>
       </c>
@@ -1299,6 +1401,9 @@
         <v>17</v>
       </c>
       <c r="B72" s="2"/>
+      <c r="C72" t="s">
+        <v>88</v>
+      </c>
       <c r="D72" t="s">
         <v>91</v>
       </c>
@@ -1308,6 +1413,9 @@
         <v>34</v>
       </c>
       <c r="B73" s="2"/>
+      <c r="C73" t="s">
+        <v>88</v>
+      </c>
       <c r="D73" t="s">
         <v>91</v>
       </c>
@@ -1329,6 +1437,9 @@
         <v>27</v>
       </c>
       <c r="B76" s="2"/>
+      <c r="C76" t="s">
+        <v>88</v>
+      </c>
       <c r="D76" t="s">
         <v>91</v>
       </c>
@@ -1350,6 +1461,9 @@
         <v>19</v>
       </c>
       <c r="B78" s="2"/>
+      <c r="C78" t="s">
+        <v>88</v>
+      </c>
       <c r="D78" t="s">
         <v>91</v>
       </c>
@@ -1357,6 +1471,10 @@
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>73</v>
+      </c>
+      <c r="B79" s="3"/>
+      <c r="C79" t="s">
+        <v>88</v>
       </c>
       <c r="D79" t="s">
         <v>91</v>

</xml_diff>